<commit_message>
Robot 15 Creating Random CV's
-> Creates random CV's using ChatGPT and write that data on a Word file
</commit_message>
<xml_diff>
--- a/Robot4_RealEstateWebScraping/PropertyListings.xlsx
+++ b/Robot4_RealEstateWebScraping/PropertyListings.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Course\UiPathRobots\Robot4_RealEstateWebScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF73F9D-7ED3-41D1-845A-967417769B86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C00714-3334-4907-AD21-285ED5C5BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6DDA14DA-8800-4BCF-813B-9F771BCBEEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW YORK" sheetId="13" r:id="rId1"/>
-    <sheet name="TEXAS" sheetId="14" r:id="rId2"/>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId3"/>
+    <sheet name="WASHINGTON" sheetId="16" r:id="rId2"/>
+    <sheet name="TEXAS" sheetId="14" r:id="rId3"/>
+    <sheet name="Sayfa1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="405">
   <si>
     <t>Price</t>
   </si>
@@ -840,6 +841,408 @@
   </si>
   <si>
     <t>Lumberton</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4128-E-Longfellow-Ave-Spokane-WA-99217/23505289_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3736-Cartier-Dr-Bremerton-WA-98312/70998687_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/8900-Saint-Helens-Ave-Vancouver-WA-98664/23240192_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/18905-8th-Ave-SW-Normandy-Park-WA-98166/48982660_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4818-N-Wall-St-Spokane-WA-99205/23551974_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/22-Brian-Rd-Washougal-WA-98671/90129538_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/22726-Trails-End-Rd-SE-Yelm-WA-98597/49386930_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/14071-117th-Ave-NE-Kirkland-WA-98034/48857326_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/13511-NE-79th-Cir-Vancouver-WA-98682/23270955_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/5934-N-Moore-St-Spokane-WA-99205/23492857_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9722-62nd-Ave-SE-Olympia-WA-98513/49367364_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1919-Gregory-Way-Bremerton-WA-98337/23422713_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1955-Rainier-Ave-Bremerton-WA-98312/23402778_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/351-Holcomb-Spur-Rd-Kelso-WA-98626/67029873_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1295-NW-Elford-Dr-Seattle-WA-98177/48790962_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/304-Orting-Ct-NW-Orting-WA-98360/49307671_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2151-W-4th-St-Port-Angeles-WA-98363/114645240_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3321-Harris-Rd-SE-Pt-Orchard-WA-98366/71558088_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/25500-N-Wenas-Rd-Selah-WA-98942/333768759_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1709-Stuart-St-Walla-Walla-WA-99362/91572421_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1332-E-29th-Ave-Spokane-WA-99203/23535578_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2971-Longhorn-Loop-277-Ellensburg-WA-98926/2054154812_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/504-S-Ray-St-Spokane-WA-99202/23525015_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1817-W-7th-Pl-Kennewick-WA-99336/85948116_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/8505-Midvale-Rd-Yakima-WA-98908/80128944_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2574-Highline-Rd-Chewelah-WA-99109/108187420_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/319111-2nd-Hwy-Newport-WA-99156/2057752060_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/645-NW-137th-St-Seattle-WA-98177/48798497_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3313-S-Fancher-Rd-Spokane-WA-99223/23540696_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1022-9th-St-SW-Puyallup-WA-98371/49272251_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/11416-Prairie-Ct-SE-Olympia-WA-98513/49386066_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/581-Cherry-St-Blaine-WA-98230/23648187_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2607-NW-Carty-Rd-Ridgefield-WA-98642/23324902_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4416-127th-St-NE-Marysville-WA-98271/38554007_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/401-E-Lakeshore-Dr-Allyn-WA-98524/72066836_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2335-Terrace-St-Bremerton-WA-98310/23426458_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1485-Whittier-Ave-SE-Port-Orchard-WA-98366/23443768_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/13001-NE-55th-Ave-Vancouver-WA-98686/328530319_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/17042-431st-Ave-SE-North-Bend-WA-98045/49132909_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/109-Ross-Canyon-Rd-Omak-WA-98841/102640817_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9490-SE-47th-St-Mercer-Island-WA-98040/48767389_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/13225-112th-Ave-NE-Kirkland-WA-98034/49000395_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/24820-11th-Ave-S-Des-Moines-WA-98198/48879543_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4778-Village-View-St-Richland-WA-99352/2055893291_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9204-15th-St-SE-Lake-Stevens-WA-98258/38577902_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/959-10th-St-Washougal-WA-98671/67684250_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/515-15th-St-NE-East-Wenatchee-WA-98802/79357805_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/103-Milwaukee-St-Mount-Vernon-WA-98273/2054246332_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/26710-NE-Ring-St-Duvall-WA-98019/48780743_zpid/</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/7861-Amethyst-Loop-NW-Silverdale-WA-98383/23458717_zpid/</t>
+  </si>
+  <si>
+    <t>4128 E Longfellow Ave</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>3736 NW Cartier Drive</t>
+  </si>
+  <si>
+    <t>Bremerton</t>
+  </si>
+  <si>
+    <t>8900 Saint Helens Ave</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>18905 8th Avenue SW</t>
+  </si>
+  <si>
+    <t>Normandy Park</t>
+  </si>
+  <si>
+    <t>4818 N Wall St</t>
+  </si>
+  <si>
+    <t>22 Brian Rd</t>
+  </si>
+  <si>
+    <t>Washougal</t>
+  </si>
+  <si>
+    <t>22726 Trails End Road SE</t>
+  </si>
+  <si>
+    <t>Yelm</t>
+  </si>
+  <si>
+    <t>14071 117th Avenue NE</t>
+  </si>
+  <si>
+    <t>Kirkland</t>
+  </si>
+  <si>
+    <t>13511 NE 79th Cir</t>
+  </si>
+  <si>
+    <t>5934 N Moore St</t>
+  </si>
+  <si>
+    <t>9722 62nd Avenue SE</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>1919 Gregory Way</t>
+  </si>
+  <si>
+    <t>1955 N Rainier Avenue</t>
+  </si>
+  <si>
+    <t>351 Holcomb Spur Road</t>
+  </si>
+  <si>
+    <t>Kelso</t>
+  </si>
+  <si>
+    <t>1295 NW Elford Drive</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>304 Orting Court NW</t>
+  </si>
+  <si>
+    <t>Orting</t>
+  </si>
+  <si>
+    <t>2151 W 4th Street</t>
+  </si>
+  <si>
+    <t>Port Angeles</t>
+  </si>
+  <si>
+    <t>3321 Harris Road SE</t>
+  </si>
+  <si>
+    <t>Port Orchard</t>
+  </si>
+  <si>
+    <t>25500 N Wenas Road</t>
+  </si>
+  <si>
+    <t>Selah</t>
+  </si>
+  <si>
+    <t>1709 Stuart Street</t>
+  </si>
+  <si>
+    <t>Walla Walla</t>
+  </si>
+  <si>
+    <t>1332 E 29th Ave</t>
+  </si>
+  <si>
+    <t>2971 Longhorn Loop UNIT 277</t>
+  </si>
+  <si>
+    <t>Ellensburg</t>
+  </si>
+  <si>
+    <t>504 S Ray St</t>
+  </si>
+  <si>
+    <t>1817 W 7th Pl</t>
+  </si>
+  <si>
+    <t>Kennewick</t>
+  </si>
+  <si>
+    <t>8505 Midvale Rd</t>
+  </si>
+  <si>
+    <t>Yakima</t>
+  </si>
+  <si>
+    <t>2574 Highline Rd</t>
+  </si>
+  <si>
+    <t>Chewelah</t>
+  </si>
+  <si>
+    <t>319111 2nd Hwy</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>645 NW 137th Street</t>
+  </si>
+  <si>
+    <t>3313 S Fancher Rd</t>
+  </si>
+  <si>
+    <t>1022 9th Street SW</t>
+  </si>
+  <si>
+    <t>Puyallup</t>
+  </si>
+  <si>
+    <t>11416 Prairie Court SE</t>
+  </si>
+  <si>
+    <t>581 Cherry Street</t>
+  </si>
+  <si>
+    <t>Blaine</t>
+  </si>
+  <si>
+    <t>2607 NW Carty Road</t>
+  </si>
+  <si>
+    <t>Ridgefield</t>
+  </si>
+  <si>
+    <t>4416 127th Street NE</t>
+  </si>
+  <si>
+    <t>Marysville</t>
+  </si>
+  <si>
+    <t>401 E Lakeshore Drive</t>
+  </si>
+  <si>
+    <t>Allyn</t>
+  </si>
+  <si>
+    <t>2335 Terrace Street</t>
+  </si>
+  <si>
+    <t>1485 Whittier Avenue SE</t>
+  </si>
+  <si>
+    <t>13001 NE 55th Ave</t>
+  </si>
+  <si>
+    <t>17042 431st Avenue SE</t>
+  </si>
+  <si>
+    <t>North Bend</t>
+  </si>
+  <si>
+    <t>109 Ross Canyon Road</t>
+  </si>
+  <si>
+    <t>Omak</t>
+  </si>
+  <si>
+    <t>9490 SE 47th Street</t>
+  </si>
+  <si>
+    <t>Mercer Island</t>
+  </si>
+  <si>
+    <t>13225 112th Avenue NE</t>
+  </si>
+  <si>
+    <t>24820 11th Avenue S</t>
+  </si>
+  <si>
+    <t>Des Moines</t>
+  </si>
+  <si>
+    <t>4778 Village View Street</t>
+  </si>
+  <si>
+    <t>Richland</t>
+  </si>
+  <si>
+    <t>9204 15th St SE</t>
+  </si>
+  <si>
+    <t>Lake Stevens</t>
+  </si>
+  <si>
+    <t>959 10th St</t>
+  </si>
+  <si>
+    <t>515 15th Street NE</t>
+  </si>
+  <si>
+    <t>East Wenatchee</t>
+  </si>
+  <si>
+    <t>103 Milwaukee Street</t>
+  </si>
+  <si>
+    <t>26710 NE Ring Street</t>
+  </si>
+  <si>
+    <t>Duvall</t>
+  </si>
+  <si>
+    <t>7861 Amethyst Loop NW</t>
+  </si>
+  <si>
+    <t>Silverdale</t>
   </si>
 </sst>
 </file>
@@ -884,11 +1287,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2645,10 +3049,1511 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605BDCC8-63A8-478A-B8B1-BC2A8639373F}">
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>249000</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2394</v>
+      </c>
+      <c r="E2" s="3">
+        <v>104.010025062656</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H2" s="4">
+        <v>99156</v>
+      </c>
+      <c r="I2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>225000</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2072</v>
+      </c>
+      <c r="E3" s="3">
+        <v>108.590733590733</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="4">
+        <v>98626</v>
+      </c>
+      <c r="I3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>250000</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2152</v>
+      </c>
+      <c r="E4" s="3">
+        <v>116.171003717472</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H4" s="4">
+        <v>99202</v>
+      </c>
+      <c r="I4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>269900</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2178</v>
+      </c>
+      <c r="E5" s="3">
+        <v>123.92102846648299</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H5" s="4">
+        <v>99203</v>
+      </c>
+      <c r="I5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>375000</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2900</v>
+      </c>
+      <c r="E6" s="3">
+        <v>129.31034482758599</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H6" s="4">
+        <v>98841</v>
+      </c>
+      <c r="I6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>539900</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3600</v>
+      </c>
+      <c r="E7" s="3">
+        <v>149.972222222222</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="H7" s="4">
+        <v>99109</v>
+      </c>
+      <c r="I7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>325000</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2052</v>
+      </c>
+      <c r="E8" s="3">
+        <v>158.38206627680299</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H8" s="4">
+        <v>99205</v>
+      </c>
+      <c r="I8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>360000</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2233</v>
+      </c>
+      <c r="E9" s="3">
+        <v>161.21809225257499</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="4">
+        <v>99205</v>
+      </c>
+      <c r="I9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>319900</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1984</v>
+      </c>
+      <c r="E10" s="3">
+        <v>161.23991935483801</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H10" s="4">
+        <v>99217</v>
+      </c>
+      <c r="I10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>559000</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3178</v>
+      </c>
+      <c r="E11" s="3">
+        <v>175.89679043423499</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H11" s="4">
+        <v>98366</v>
+      </c>
+      <c r="I11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>369000</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1950</v>
+      </c>
+      <c r="E12" s="3">
+        <v>189.230769230769</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H12" s="4">
+        <v>99362</v>
+      </c>
+      <c r="I12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>340000</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1702</v>
+      </c>
+      <c r="E13" s="3">
+        <v>199.76498237367801</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H13" s="4">
+        <v>99336</v>
+      </c>
+      <c r="I13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>499995</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2417</v>
+      </c>
+      <c r="E14" s="3">
+        <v>206.86594952420299</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H14" s="4">
+        <v>98310</v>
+      </c>
+      <c r="I14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>695000</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>3300</v>
+      </c>
+      <c r="E15" s="3">
+        <v>210.60606060606</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H15" s="4">
+        <v>98802</v>
+      </c>
+      <c r="I15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>445000</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2010</v>
+      </c>
+      <c r="E16" s="3">
+        <v>221.39303482586999</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H16" s="4">
+        <v>98908</v>
+      </c>
+      <c r="I16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>730000</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3286</v>
+      </c>
+      <c r="E17" s="3">
+        <v>222.15459525258601</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H17" s="4">
+        <v>99223</v>
+      </c>
+      <c r="I17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>349000</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1450</v>
+      </c>
+      <c r="E18" s="3">
+        <v>240.68965517241301</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="4">
+        <v>98273</v>
+      </c>
+      <c r="I18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>499900</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2061</v>
+      </c>
+      <c r="E19" s="3">
+        <v>242.552159146045</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="H19" s="4">
+        <v>98230</v>
+      </c>
+      <c r="I19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>389500</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>1542</v>
+      </c>
+      <c r="E20" s="3">
+        <v>252.59403372243801</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H20" s="4">
+        <v>98312</v>
+      </c>
+      <c r="I20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>384995</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1497</v>
+      </c>
+      <c r="E21" s="3">
+        <v>257.17768871075401</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H21" s="4">
+        <v>98926</v>
+      </c>
+      <c r="I21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>389900</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>1516</v>
+      </c>
+      <c r="E22" s="3">
+        <v>257.189973614775</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H22" s="4">
+        <v>98513</v>
+      </c>
+      <c r="I22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>825000</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3180</v>
+      </c>
+      <c r="E23" s="3">
+        <v>259.43396226415001</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H23" s="4">
+        <v>98166</v>
+      </c>
+      <c r="I23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>395000</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1480</v>
+      </c>
+      <c r="E24" s="3">
+        <v>266.89189189189102</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H24" s="4">
+        <v>98337</v>
+      </c>
+      <c r="I24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>599999</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2236</v>
+      </c>
+      <c r="E25" s="3">
+        <v>268.335867620751</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H25" s="4">
+        <v>98258</v>
+      </c>
+      <c r="I25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>724900</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>2639</v>
+      </c>
+      <c r="E26" s="3">
+        <v>274.68738158393302</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H26" s="4">
+        <v>98363</v>
+      </c>
+      <c r="I26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>470000</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1704</v>
+      </c>
+      <c r="E27" s="3">
+        <v>275.821596244131</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H27" s="4">
+        <v>99352</v>
+      </c>
+      <c r="I27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>495000</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>1768</v>
+      </c>
+      <c r="E28" s="3">
+        <v>279.97737556560998</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H28" s="4">
+        <v>98524</v>
+      </c>
+      <c r="I28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>350000</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1242</v>
+      </c>
+      <c r="E29" s="3">
+        <v>281.80354267310702</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H29" s="4">
+        <v>98682</v>
+      </c>
+      <c r="I29" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>525000</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1812</v>
+      </c>
+      <c r="E30" s="3">
+        <v>289.73509933774801</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H30" s="4">
+        <v>98271</v>
+      </c>
+      <c r="I30" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>580000</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1874</v>
+      </c>
+      <c r="E31" s="3">
+        <v>309.498399146211</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H31" s="4">
+        <v>98371</v>
+      </c>
+      <c r="I31" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>610000</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>1950</v>
+      </c>
+      <c r="E32" s="3">
+        <v>312.82051282051202</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H32" s="4">
+        <v>98383</v>
+      </c>
+      <c r="I32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>449000</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1424</v>
+      </c>
+      <c r="E33" s="3">
+        <v>315.30898876404399</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H33" s="4">
+        <v>98664</v>
+      </c>
+      <c r="I33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>789950</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2404</v>
+      </c>
+      <c r="E34" s="3">
+        <v>328.59816971713798</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H34" s="4">
+        <v>98513</v>
+      </c>
+      <c r="I34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>585000</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>1760</v>
+      </c>
+      <c r="E35" s="3">
+        <v>332.386363636363</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H35" s="4">
+        <v>98671</v>
+      </c>
+      <c r="I35" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>595000</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>1760</v>
+      </c>
+      <c r="E36" s="3">
+        <v>338.06818181818102</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H36" s="4">
+        <v>98942</v>
+      </c>
+      <c r="I36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>539000</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1581</v>
+      </c>
+      <c r="E37" s="3">
+        <v>340.92346616065697</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H37" s="4">
+        <v>98312</v>
+      </c>
+      <c r="I37" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>749997</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>2193</v>
+      </c>
+      <c r="E38" s="3">
+        <v>341.99589603283101</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H38" s="4">
+        <v>98642</v>
+      </c>
+      <c r="I38" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>469950</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>1360</v>
+      </c>
+      <c r="E39" s="3">
+        <v>345.55147058823502</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H39" s="4">
+        <v>98360</v>
+      </c>
+      <c r="I39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>735500</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>2127</v>
+      </c>
+      <c r="E40" s="3">
+        <v>345.79219558062999</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H40" s="4">
+        <v>98686</v>
+      </c>
+      <c r="I40" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>399000</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1100</v>
+      </c>
+      <c r="E41" s="3">
+        <v>362.72727272727201</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H41" s="4">
+        <v>98366</v>
+      </c>
+      <c r="I41" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>249000</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>680</v>
+      </c>
+      <c r="E42" s="3">
+        <v>366.17647058823502</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H42" s="4">
+        <v>98597</v>
+      </c>
+      <c r="I42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>439000</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1040</v>
+      </c>
+      <c r="E43" s="3">
+        <v>422.11538461538402</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H43" s="4">
+        <v>98198</v>
+      </c>
+      <c r="I43" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>775000</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1600</v>
+      </c>
+      <c r="E44" s="3">
+        <v>484.375</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H44" s="4">
+        <v>98019</v>
+      </c>
+      <c r="I44" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>625000</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1250</v>
+      </c>
+      <c r="E45" s="3">
+        <v>500</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H45" s="4">
+        <v>98045</v>
+      </c>
+      <c r="I45" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>889950</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>1730</v>
+      </c>
+      <c r="E46" s="3">
+        <v>514.42196531791899</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H46" s="4">
+        <v>98671</v>
+      </c>
+      <c r="I46" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1599000</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>3010</v>
+      </c>
+      <c r="E47" s="3">
+        <v>531.22923588039805</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H47" s="4">
+        <v>98040</v>
+      </c>
+      <c r="I47" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>949999</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>1760</v>
+      </c>
+      <c r="E48" s="3">
+        <v>539.77215909090899</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H48" s="4">
+        <v>98034</v>
+      </c>
+      <c r="I48" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1075000</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>1950</v>
+      </c>
+      <c r="E49" s="3">
+        <v>551.28205128205104</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H49" s="4">
+        <v>98034</v>
+      </c>
+      <c r="I49" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>6000000</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>5820</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1030.9278350515399</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H50" s="4">
+        <v>98177</v>
+      </c>
+      <c r="I50" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11750000</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>7362</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1596.0336864982301</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H51" s="4">
+        <v>98177</v>
+      </c>
+      <c r="I51" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I51">
+    <sortCondition ref="E1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCE3AD5-51FB-4E94-B586-D0AD6E585DB1}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4145,7 +6050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1269A56-65E8-4394-88AF-29D7FE957770}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>